<commit_message>
doc : README.md backend reamme 파일 수정 요구사항 정의서 수정 ERD -> DBdiagram.png로 변경
</commit_message>
<xml_diff>
--- a/back/Library 프로젝트 요구사항 정의서.xlsx
+++ b/back/Library 프로젝트 요구사항 정의서.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Desktop\library project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Desktop\library project\back\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="143">
   <si>
     <t>요구사항 ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -374,21 +374,6 @@
   </si>
   <si>
     <t>SEARCH { PUBLISHER }</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>KEYWORD 를 포함한 GET 요청을 통해 
-제목에 키워드를 포함한 BOOK 데이터 LIST 를 요청 할 수 있다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>AUTHOR 를 포함한 GET 요청을 통해 
-특정 저자의 BOOK 데이터 LIST 를 요청 할 수 있다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>PUBLISHER 를 포함한 GET 요청을 통해 
-특정 출판사의 BOOK 데이터 LIST 를 요청 할 수 있다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -486,6 +471,112 @@
   </si>
   <si>
     <t>-</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>KEYWORD 를 포함한 BOOK GET 요청을 통해 
+제목에 키워드를 포함한 BOOK 데이터 LIST 를 요청 할 수 있다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AUTHOR 가 일치하는 BOOK GET 요청을 통해 
+특정 저자의 BOOK 데이터 LIST 를 요청 할 수 있다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PUBLISHER 가 일치하는 BOOK GET 요청을 통해 
+특정 출판사의 BOOK 데이터 LIST 를 요청 할 수 있다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST_001</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST_002</t>
+  </si>
+  <si>
+    <t>POST_003</t>
+  </si>
+  <si>
+    <t>POST_POST</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST_PATCH</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST_GET</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST 요청을 통해 POST 을 등록 할 수 있다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PATCH 요청을 통해 POST 을 수정 할 수 있다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>GET 요청을 통해 POST 데이터 를 요청 할 수 있다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>POSTDTO.POST</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>POSTDTO.PATCH</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST_007</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST_DELETE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DELETE 요청을 통해 POST 데이터 를 삭제 할 수 있다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMMENT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMMENT_001</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMMENT_002</t>
+  </si>
+  <si>
+    <t>COMMENT_003</t>
+  </si>
+  <si>
+    <t>COMMENT_004</t>
+  </si>
+  <si>
+    <t>COMMENT_DELETE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMMENT_POST</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMMENT_PATCH</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>COMMENT_GET</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -533,7 +624,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -558,8 +649,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -582,13 +679,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -610,19 +744,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -905,10 +1060,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17"/>
@@ -938,13 +1093,13 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
@@ -1016,135 +1171,135 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="7" t="s">
-        <v>25</v>
+        <v>91</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="3" t="s">
-        <v>26</v>
+    <row r="8" spans="1:5" ht="34">
+      <c r="A8" s="5" t="s">
+        <v>92</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>35</v>
+        <v>106</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>114</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>40</v>
+        <v>107</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>22</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="3" t="s">
-        <v>27</v>
+      <c r="A9" s="5" t="s">
+        <v>93</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>32</v>
+        <v>96</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>36</v>
+        <v>108</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>41</v>
+        <v>104</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>22</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="3" t="s">
-        <v>28</v>
+      <c r="A10" s="5" t="s">
+        <v>94</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>37</v>
+        <v>109</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>24</v>
+        <v>115</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>42</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="39" customHeight="1">
-      <c r="A11" s="3" t="s">
-        <v>29</v>
+      <c r="A11" s="5" t="s">
+        <v>95</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>91</v>
+        <v>100</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>24</v>
+        <v>115</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="34">
-      <c r="A12" s="3" t="s">
-        <v>30</v>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="5" t="s">
+        <v>97</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>92</v>
+        <v>101</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>111</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>24</v>
+        <v>115</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="34">
-      <c r="A13" s="3" t="s">
-        <v>86</v>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="51">
+      <c r="A13" s="5" t="s">
+        <v>98</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>24</v>
+        <v>115</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>42</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="3" t="s">
-        <v>87</v>
+      <c r="A14" s="5" t="s">
+        <v>105</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>34</v>
+        <v>103</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>38</v>
+        <v>113</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>43</v>
+        <v>115</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>24</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="9" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
@@ -1152,346 +1307,502 @@
       <c r="E15" s="10"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>49</v>
+      <c r="A16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>55</v>
+        <v>35</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>50</v>
+      <c r="A17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>55</v>
+        <v>36</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>51</v>
+      <c r="A18" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>24</v>
+        <v>37</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="34">
-      <c r="A19" s="5" t="s">
-        <v>48</v>
+      <c r="A19" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>39</v>
+        <v>88</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>24</v>
+        <v>116</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="34" customHeight="1">
-      <c r="A20" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
+      <c r="A20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="34">
+      <c r="A21" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="22" spans="1:5" ht="17" customHeight="1">
-      <c r="A22" s="5" t="s">
-        <v>59</v>
+      <c r="A22" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>81</v>
+        <v>34</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="42.5" customHeight="1">
-      <c r="A23" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>24</v>
-      </c>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="19" customHeight="1">
+      <c r="A23" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="5" t="s">
-        <v>61</v>
+      <c r="A24" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>65</v>
+        <v>123</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>71</v>
+        <v>126</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>24</v>
+        <v>129</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="34">
-      <c r="A25" s="5" t="s">
-        <v>62</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>72</v>
+        <v>124</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>76</v>
+        <v>130</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>77</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-    </row>
-    <row r="27" spans="1:5" ht="34">
-      <c r="A27" s="5" t="s">
-        <v>79</v>
+      <c r="A26" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="3" t="s">
+        <v>131</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>84</v>
+        <v>132</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="A28" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-    </row>
-    <row r="30" spans="1:5" ht="34">
-      <c r="A30" s="5" t="s">
-        <v>95</v>
+      <c r="A29" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="3" t="s">
+        <v>136</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>117</v>
+        <v>141</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>110</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="5" t="s">
-        <v>96</v>
+      <c r="A31" s="3" t="s">
+        <v>137</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>99</v>
+        <v>142</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>107</v>
+        <v>24</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>110</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="5" t="s">
-        <v>97</v>
+      <c r="A32" s="3" t="s">
+        <v>138</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>102</v>
+        <v>139</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>118</v>
+        <v>43</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>110</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>110</v>
-      </c>
+      <c r="A33" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="15"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>104</v>
+        <v>45</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="68">
+        <v>67</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>110</v>
+        <v>46</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>106</v>
+        <v>47</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>110</v>
+        <v>69</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="34">
+      <c r="A37" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B38" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="18"/>
+    </row>
+    <row r="40" spans="1:5" ht="34">
+      <c r="A40" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="34">
+      <c r="A41" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="34">
+      <c r="A43" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+    </row>
+    <row r="45" spans="1:5" ht="34">
+      <c r="A45" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A29:E29"/>
+  <mergeCells count="8">
+    <mergeCell ref="A7:E7"/>
     <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A7:E7"/>
     <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A44:E44"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="A33:E33"/>
+    <mergeCell ref="A39:E39"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>